<commit_message>
New Letters and Numbers. Improved wait statess=
</commit_message>
<xml_diff>
--- a/LEDS.xlsx
+++ b/LEDS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Documents\Arduino\CoatofManyColours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4479C83-C8A2-4067-AE79-E34A508B23A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8365A2FC-ED58-404F-AFBF-6C9DD388C16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="-150" windowWidth="18630" windowHeight="19440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="390" windowWidth="29445" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="6" r:id="rId1"/>
@@ -18,13 +18,18 @@
     <sheet name="D" sheetId="4" r:id="rId3"/>
     <sheet name="E" sheetId="8" r:id="rId4"/>
     <sheet name="H" sheetId="10" r:id="rId5"/>
-    <sheet name="L" sheetId="12" r:id="rId6"/>
-    <sheet name="M" sheetId="2" r:id="rId7"/>
-    <sheet name="N" sheetId="11" r:id="rId8"/>
-    <sheet name="R" sheetId="1" r:id="rId9"/>
-    <sheet name="Heart" sheetId="3" r:id="rId10"/>
-    <sheet name="#1" sheetId="5" r:id="rId11"/>
-    <sheet name="T" sheetId="7" r:id="rId12"/>
+    <sheet name="I" sheetId="14" r:id="rId6"/>
+    <sheet name="L" sheetId="12" r:id="rId7"/>
+    <sheet name="M" sheetId="2" r:id="rId8"/>
+    <sheet name="O" sheetId="16" r:id="rId9"/>
+    <sheet name="N" sheetId="11" r:id="rId10"/>
+    <sheet name="R" sheetId="1" r:id="rId11"/>
+    <sheet name="S" sheetId="15" r:id="rId12"/>
+    <sheet name="T" sheetId="7" r:id="rId13"/>
+    <sheet name="Heart" sheetId="3" r:id="rId14"/>
+    <sheet name="#1" sheetId="5" r:id="rId15"/>
+    <sheet name="6" sheetId="18" r:id="rId16"/>
+    <sheet name="0" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -688,6 +693,897 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219C932C-97F4-44A0-9790-FC1777082AC2}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4">
+        <v>27</v>
+      </c>
+      <c r="E1" s="5">
+        <v>44</v>
+      </c>
+      <c r="F1" s="5">
+        <v>45</v>
+      </c>
+      <c r="G1" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43</v>
+      </c>
+      <c r="F2" s="5">
+        <v>46</v>
+      </c>
+      <c r="G2" s="7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4">
+        <v>47</v>
+      </c>
+      <c r="G3" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5">
+        <v>48</v>
+      </c>
+      <c r="G4" s="6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6">
+        <v>40</v>
+      </c>
+      <c r="F5" s="4">
+        <v>49</v>
+      </c>
+      <c r="G5" s="6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6">
+        <v>38</v>
+      </c>
+      <c r="F7" s="5">
+        <v>51</v>
+      </c>
+      <c r="G7" s="7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5">
+        <v>37</v>
+      </c>
+      <c r="F8" s="6">
+        <v>52</v>
+      </c>
+      <c r="G8" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7">
+        <v>53</v>
+      </c>
+      <c r="G9" s="6">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1">
+        <v>44</v>
+      </c>
+      <c r="F1">
+        <v>45</v>
+      </c>
+      <c r="G1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43</v>
+      </c>
+      <c r="F2">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE147CCA-8A7D-4545-8E78-1EFBD855654D}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45</v>
+      </c>
+      <c r="G1" s="9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1">
+        <v>46</v>
+      </c>
+      <c r="G2" s="9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1">
+        <v>47</v>
+      </c>
+      <c r="G3" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1">
+        <v>48</v>
+      </c>
+      <c r="G4" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>49</v>
+      </c>
+      <c r="G5" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+      <c r="G6" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9">
+        <v>51</v>
+      </c>
+      <c r="G7" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8">
+        <v>52</v>
+      </c>
+      <c r="G8" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1">
+        <v>53</v>
+      </c>
+      <c r="G9" s="8">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AC6BEE-81DA-4F6D-85EE-63FDA0350FF5}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7">
+        <v>44</v>
+      </c>
+      <c r="F1" s="7">
+        <v>45</v>
+      </c>
+      <c r="G1" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43</v>
+      </c>
+      <c r="F2" s="9">
+        <v>46</v>
+      </c>
+      <c r="G2" s="9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9">
+        <v>42</v>
+      </c>
+      <c r="F3" s="8">
+        <v>47</v>
+      </c>
+      <c r="G3" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9">
+        <v>41</v>
+      </c>
+      <c r="F4" s="9">
+        <v>48</v>
+      </c>
+      <c r="G4" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6">
+        <v>31</v>
+      </c>
+      <c r="E5" s="8">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8">
+        <v>49</v>
+      </c>
+      <c r="G5" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+      <c r="G6" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9">
+        <v>51</v>
+      </c>
+      <c r="G7" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8">
+        <v>52</v>
+      </c>
+      <c r="G8" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7">
+        <v>35</v>
+      </c>
+      <c r="E9" s="9">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9">
+        <v>53</v>
+      </c>
+      <c r="G9" s="8">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -909,7 +1805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1132,225 +2028,459 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AC6BEE-81DA-4F6D-85EE-63FDA0350FF5}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667F8E8F-3A37-4ED8-B47F-45A793E58395}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6">
+    <row r="1" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>8</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
         <v>9</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="1">
         <v>26</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="1">
         <v>27</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="1">
         <v>44</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1">
         <v>45</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>7</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2">
         <v>28</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2">
         <v>43</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="1">
         <v>46</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>6</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <v>24</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
         <v>29</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3">
         <v>42</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3">
         <v>47</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+    <row r="4" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4">
         <v>23</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4">
         <v>41</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4">
         <v>48</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>13</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="1">
         <v>22</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>31</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="1">
         <v>40</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5">
         <v>49</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="1">
         <v>14</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6">
         <v>21</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>32</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>39</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="1">
         <v>50</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>15</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7">
         <v>33</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>38</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7">
         <v>51</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="1">
         <v>16</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8">
         <v>19</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8">
         <v>34</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8">
         <v>37</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="1">
         <v>52</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>0</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>17</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="1">
         <v>18</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="1">
         <v>35</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="1">
         <v>36</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
         <v>53</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925F8033-8DF4-48D7-AAAF-98CF509B3E69}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44</v>
+      </c>
+      <c r="F1">
+        <v>45</v>
+      </c>
+      <c r="G1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1358,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521B3BD8-3505-4918-AE55-14CC576B3A7C}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +2498,7 @@
       <c r="A1" s="4">
         <v>8</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
         <v>9</v>
       </c>
       <c r="C1" s="6">
@@ -1391,7 +2521,7 @@
       <c r="A2" s="4">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
       <c r="C2" s="5">
@@ -1411,10 +2541,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="1">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3">
         <v>11</v>
       </c>
       <c r="C3" s="5">
@@ -1434,10 +2564,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4">
         <v>12</v>
       </c>
       <c r="C4" s="5">
@@ -1457,10 +2587,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>13</v>
       </c>
       <c r="C5" s="4">
@@ -1480,10 +2610,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6">
         <v>14</v>
       </c>
       <c r="C6" s="5">
@@ -1503,10 +2633,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7">
         <v>15</v>
       </c>
       <c r="C7" s="5">
@@ -1529,7 +2659,7 @@
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="1">
         <v>16</v>
       </c>
       <c r="C8" s="5">
@@ -1552,7 +2682,7 @@
       <c r="A9" s="4">
         <v>0</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9">
         <v>17</v>
       </c>
       <c r="C9" s="7">
@@ -1581,7 +2711,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,10 +3384,236 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE765DC-2DA4-44A7-BD97-6164DF7A373A}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44</v>
+      </c>
+      <c r="F1" s="9">
+        <v>45</v>
+      </c>
+      <c r="G1" s="9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43</v>
+      </c>
+      <c r="F2" s="9">
+        <v>46</v>
+      </c>
+      <c r="G2" s="9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9">
+        <v>42</v>
+      </c>
+      <c r="F3" s="8">
+        <v>47</v>
+      </c>
+      <c r="G3" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9">
+        <v>41</v>
+      </c>
+      <c r="F4" s="9">
+        <v>48</v>
+      </c>
+      <c r="G4" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>31</v>
+      </c>
+      <c r="E5" s="8">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8">
+        <v>49</v>
+      </c>
+      <c r="G5" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+      <c r="G6" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9">
+        <v>51</v>
+      </c>
+      <c r="G7" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8">
+        <v>52</v>
+      </c>
+      <c r="G8" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9">
+        <v>53</v>
+      </c>
+      <c r="G9" s="8">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DB7004-0E6A-4CB4-B37A-F33755E2BC74}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2475,7 +3831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -2698,36 +4054,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219C932C-97F4-44A0-9790-FC1777082AC2}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB158F02-F30C-4B58-B151-CE996E32EA1C}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>8</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
         <v>9</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="1">
         <v>26</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="1">
         <v>27</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="1">
         <v>44</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1">
         <v>45</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="5">
         <v>62</v>
       </c>
     </row>
@@ -2735,10 +4094,10 @@
       <c r="A2" s="4">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>25</v>
       </c>
       <c r="D2" s="5">
@@ -2747,10 +4106,10 @@
       <c r="E2" s="4">
         <v>43</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="1">
         <v>46</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <v>61</v>
       </c>
     </row>
@@ -2758,22 +4117,22 @@
       <c r="A3" s="4">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="1">
         <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>24</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>29</v>
       </c>
       <c r="E3" s="5">
         <v>42</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>47</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>60</v>
       </c>
     </row>
@@ -2781,22 +4140,22 @@
       <c r="A4" s="4">
         <v>5</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="1">
         <v>12</v>
       </c>
       <c r="C4" s="5">
         <v>23</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>30</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>41</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="1">
         <v>48</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>59</v>
       </c>
     </row>
@@ -2804,22 +4163,22 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="1">
         <v>13</v>
       </c>
       <c r="C5" s="4">
         <v>22</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>31</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>40</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>49</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>58</v>
       </c>
     </row>
@@ -2827,7 +4186,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="1">
         <v>14</v>
       </c>
       <c r="C6" s="5">
@@ -2836,13 +4195,13 @@
       <c r="D6" s="4">
         <v>32</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>39</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="1">
         <v>50</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>57</v>
       </c>
     </row>
@@ -2850,7 +4209,7 @@
       <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="1">
         <v>15</v>
       </c>
       <c r="C7" s="5">
@@ -2859,13 +4218,13 @@
       <c r="D7" s="5">
         <v>33</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>38</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="1">
         <v>51</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>56</v>
       </c>
     </row>
@@ -2873,7 +4232,7 @@
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="1">
         <v>16</v>
       </c>
       <c r="C8" s="5">
@@ -2885,10 +4244,10 @@
       <c r="E8" s="5">
         <v>37</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="1">
         <v>52</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>55</v>
       </c>
     </row>
@@ -2896,248 +4255,27 @@
       <c r="A9" s="4">
         <v>0</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9">
         <v>17</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="1">
         <v>18</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="1">
         <v>35</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="1">
         <v>36</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9">
         <v>53</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1">
-        <v>44</v>
-      </c>
-      <c r="F1">
-        <v>45</v>
-      </c>
-      <c r="G1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1">
-        <v>43</v>
-      </c>
-      <c r="F2">
-        <v>46</v>
-      </c>
-      <c r="G2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <v>29</v>
-      </c>
-      <c r="E3">
-        <v>42</v>
-      </c>
-      <c r="F3" s="1">
-        <v>47</v>
-      </c>
-      <c r="G3" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>41</v>
-      </c>
-      <c r="F4">
-        <v>48</v>
-      </c>
-      <c r="G4" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>39</v>
-      </c>
-      <c r="F6">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1">
-        <v>38</v>
-      </c>
-      <c r="F7">
-        <v>51</v>
-      </c>
-      <c r="G7">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>34</v>
-      </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1">
-        <v>52</v>
-      </c>
-      <c r="G8">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>35</v>
-      </c>
-      <c r="E9">
-        <v>36</v>
-      </c>
-      <c r="F9">
-        <v>53</v>
-      </c>
-      <c r="G9" s="1">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>